<commit_message>
make block size derivable
</commit_message>
<xml_diff>
--- a/example/output_files/319meeting.xlsx
+++ b/example/output_files/319meeting.xlsx
@@ -114,13 +114,6 @@
       <sz val="9"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <b val="1"/>
-      <sz val="10"/>
-    </font>
-    <font>
       <name val="宋体"/>
       <charset val="134"/>
       <family val="3"/>
@@ -136,6 +129,13 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="1"/>
       <sz val="10"/>
@@ -415,6 +415,17 @@
     </border>
     <border>
       <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -428,17 +439,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
@@ -534,7 +534,7 @@
     <xf applyAlignment="1" borderId="9" fillId="3" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="9" fillId="3" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="9" fillId="3" fontId="18" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="12" fillId="0" fontId="14" numFmtId="20" pivotButton="0" quotePrefix="0" xfId="0">
@@ -551,7 +551,7 @@
     <xf applyAlignment="1" borderId="12" fillId="0" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="12" fillId="0" fontId="16" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="12" fillId="0" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="18" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -560,25 +560,25 @@
     <xf applyAlignment="1" borderId="12" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="21" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="12" fillId="3" fontId="17" numFmtId="20" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="20" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="12" fillId="3" fontId="16" numFmtId="20" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="12" fillId="3" fontId="16" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="12" fillId="3" fontId="17" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="12" fillId="3" fontId="17" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="12" fillId="3" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf applyAlignment="1" borderId="12" fillId="3" fontId="18" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="12" fillId="3" fontId="18" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="12" fillId="3" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="12" fillId="3" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf applyAlignment="1" borderId="12" fillId="0" fontId="14" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -588,21 +588,21 @@
     <xf applyAlignment="1" borderId="12" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="12" fillId="0" fontId="16" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="12" fillId="4" fontId="16" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="12" fillId="5" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="12" fillId="6" fontId="16" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf applyAlignment="1" borderId="12" fillId="0" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="12" fillId="4" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="12" fillId="5" fontId="18" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="12" fillId="6" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="12" fillId="0" fontId="18" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf applyAlignment="1" borderId="12" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -612,10 +612,10 @@
     <xf applyAlignment="1" borderId="12" fillId="0" fontId="21" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="12" fillId="3" fontId="16" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="12" fillId="3" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="20" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="21" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -3012,8 +3012,8 @@
     <mergeCell ref="A35:F35"/>
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="K49:L49"/>
+    <mergeCell ref="A25:F25"/>
     <mergeCell ref="K24:N24"/>
-    <mergeCell ref="A25:F25"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="A44:F44"/>

</xml_diff>